<commit_message>
Updated bootstrap Cap to 100V
Forgot to upgrade bootstrapping capacitor to 100V as well...
</commit_message>
<xml_diff>
--- a/Outputs/BOM A1.xlsx
+++ b/Outputs/BOM A1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thollis\Google Drive\Motor_Controller\Outputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BA58921-C529-490A-A11E-626BE9D5FA46}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DB86709-6A76-4BA4-949F-C4125DF70028}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{8C68834D-B67F-41EE-AAEA-B755F81D1523}"/>
   </bookViews>
@@ -16,8 +16,8 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$6:$H$53</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$H$22</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$6:$H$54</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$H$23</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="72">
   <si>
     <t>Bill of Materials</t>
   </si>
@@ -265,6 +265,18 @@
   </si>
   <si>
     <t>Schottky diode, 100V 2A</t>
+  </si>
+  <si>
+    <t>C5, C6</t>
+  </si>
+  <si>
+    <t>220N</t>
+  </si>
+  <si>
+    <t>Unpolarized capacitor, 100V</t>
+  </si>
+  <si>
+    <t>587-5013-1-ND</t>
   </si>
 </sst>
 </file>
@@ -727,10 +739,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{977BF482-39EA-4C0A-A239-7A9BCEF8ADE8}">
-  <dimension ref="A1:H53"/>
+  <dimension ref="A1:H54"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -789,13 +801,13 @@
         <v>10</v>
       </c>
       <c r="F4" s="10">
-        <f>SUM(F7:F53)</f>
-        <v>27</v>
+        <f>SUM(F7:F54)</f>
+        <v>29</v>
       </c>
       <c r="G4" s="10"/>
       <c r="H4" s="11">
-        <f>SUM(H7:H53)</f>
-        <v>21.08</v>
+        <f>SUM(H7:H54)</f>
+        <v>21.599999999999998</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -852,7 +864,7 @@
         <v>0.1</v>
       </c>
       <c r="H7" s="6">
-        <f t="shared" ref="H7:H16" si="0">G7*F7</f>
+        <f t="shared" ref="H7:H17" si="0">G7*F7</f>
         <v>0.2</v>
       </c>
     </row>
@@ -908,98 +920,98 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>35</v>
+        <v>68</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="D10" s="7"/>
       <c r="E10" s="7" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="F10" s="14">
         <v>2</v>
       </c>
       <c r="G10" s="6">
-        <v>0.43</v>
+        <v>0.26</v>
       </c>
       <c r="H10" s="6">
         <f t="shared" si="0"/>
-        <v>0.86</v>
+        <v>0.52</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>8</v>
+        <v>35</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>41</v>
+        <v>66</v>
       </c>
       <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
+      <c r="E11" s="7" t="s">
+        <v>65</v>
+      </c>
       <c r="F11" s="14">
-        <v>1</v>
-      </c>
-      <c r="G11" s="6"/>
+        <v>2</v>
+      </c>
+      <c r="G11" s="6">
+        <v>0.43</v>
+      </c>
       <c r="H11" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.86</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>61</v>
+        <v>41</v>
       </c>
       <c r="D12" s="7"/>
-      <c r="E12" s="7" t="s">
-        <v>59</v>
-      </c>
+      <c r="E12" s="7"/>
       <c r="F12" s="14">
-        <v>4</v>
-      </c>
-      <c r="G12" s="6">
-        <v>1.79</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="G12" s="6"/>
       <c r="H12" s="6">
         <f t="shared" si="0"/>
-        <v>7.16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>9</v>
+        <v>60</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>17</v>
+        <v>61</v>
       </c>
       <c r="D13" s="7"/>
       <c r="E13" s="7" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="F13" s="14">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G13" s="6">
-        <v>0.1</v>
+        <v>1.79</v>
       </c>
       <c r="H13" s="6">
         <f t="shared" si="0"/>
-        <v>0.2</v>
+        <v>7.16</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -1007,14 +1019,14 @@
         <v>9</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D14" s="7"/>
       <c r="E14" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F14" s="14">
         <v>2</v>
@@ -1032,24 +1044,24 @@
         <v>9</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D15" s="7"/>
       <c r="E15" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F15" s="14">
         <v>2</v>
       </c>
       <c r="G15" s="6">
-        <v>0.13</v>
+        <v>0.1</v>
       </c>
       <c r="H15" s="6">
         <f t="shared" si="0"/>
-        <v>0.26</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -1057,24 +1069,24 @@
         <v>9</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>42</v>
+        <v>19</v>
       </c>
       <c r="D16" s="7"/>
       <c r="E16" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F16" s="14">
         <v>2</v>
       </c>
       <c r="G16" s="6">
-        <v>0.1</v>
+        <v>0.13</v>
       </c>
       <c r="H16" s="6">
         <f t="shared" si="0"/>
-        <v>0.2</v>
+        <v>0.26</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -1082,156 +1094,173 @@
         <v>9</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D17" s="7"/>
       <c r="E17" s="7" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="F17" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G17" s="6">
-        <v>1.52</v>
+        <v>0.1</v>
       </c>
       <c r="H17" s="6">
-        <f>G17*F17</f>
-        <v>1.52</v>
+        <f t="shared" si="0"/>
+        <v>0.2</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>45</v>
+        <v>9</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="D18" s="7"/>
       <c r="E18" s="7" t="s">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="F18" s="14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G18" s="6">
-        <v>3.03</v>
+        <v>1.52</v>
       </c>
       <c r="H18" s="6">
-        <f>F18*G18</f>
-        <v>6.06</v>
+        <f>G18*F18</f>
+        <v>1.52</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>57</v>
+        <v>26</v>
       </c>
       <c r="D19" s="7"/>
       <c r="E19" s="7" t="s">
-        <v>56</v>
+        <v>25</v>
       </c>
       <c r="F19" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G19" s="6">
-        <v>0.52</v>
+        <v>3.03</v>
       </c>
       <c r="H19" s="6">
-        <f t="shared" ref="H19:H22" si="1">F19*G19</f>
-        <v>0.52</v>
+        <f>F19*G19</f>
+        <v>6.06</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>32</v>
+        <v>57</v>
       </c>
       <c r="D20" s="7"/>
       <c r="E20" s="7" t="s">
-        <v>33</v>
+        <v>56</v>
       </c>
       <c r="F20" s="14">
         <v>1</v>
       </c>
       <c r="G20" s="6">
+        <v>0.52</v>
+      </c>
+      <c r="H20" s="6">
+        <f t="shared" ref="H20:H23" si="1">F20*G20</f>
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>48</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="F21" s="14">
+        <v>1</v>
+      </c>
+      <c r="G21" s="6">
         <v>0.51</v>
       </c>
-      <c r="H20" s="6">
+      <c r="H21" s="6">
         <f t="shared" si="1"/>
         <v>0.51</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>49</v>
       </c>
-      <c r="B21" s="14" t="s">
+      <c r="B22" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="C21" s="14" t="s">
+      <c r="C22" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7" t="s">
+      <c r="D22" s="7"/>
+      <c r="E22" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="F21" s="14">
+      <c r="F22" s="14">
         <v>1</v>
       </c>
-      <c r="G21" s="6">
+      <c r="G22" s="6">
         <v>0.46</v>
       </c>
-      <c r="H21" s="6">
+      <c r="H22" s="6">
         <f t="shared" si="1"/>
         <v>0.46</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>64</v>
       </c>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5" t="s">
+      <c r="B23" s="5"/>
+      <c r="C23" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7" t="s">
+      <c r="D23" s="7"/>
+      <c r="E23" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="F22" s="14">
+      <c r="F23" s="14">
         <v>2</v>
       </c>
-      <c r="G22" s="6">
+      <c r="G23" s="6">
         <v>0.36</v>
       </c>
-      <c r="H22" s="6">
+      <c r="H23" s="6">
         <f t="shared" si="1"/>
         <v>0.72</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B24" s="5"/>
@@ -1251,14 +1280,14 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="7"/>
       <c r="E26" s="7"/>
       <c r="G26" s="6"/>
       <c r="H26" s="6"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B27" s="5"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="7"/>
       <c r="E27" s="7"/>
       <c r="G27" s="6"/>
       <c r="H27" s="6"/>
@@ -1471,8 +1500,16 @@
       <c r="G53" s="6"/>
       <c r="H53" s="6"/>
     </row>
+    <row r="54" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B54" s="5"/>
+      <c r="C54" s="5"/>
+      <c r="D54" s="7"/>
+      <c r="E54" s="7"/>
+      <c r="G54" s="6"/>
+      <c r="H54" s="6"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A6:H53" xr:uid="{D36DBF69-DC81-4CC3-9038-6D644FA24F43}"/>
+  <autoFilter ref="A6:H54" xr:uid="{D36DBF69-DC81-4CC3-9038-6D644FA24F43}"/>
   <mergeCells count="3">
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A2:C2"/>
@@ -1482,18 +1519,12 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="52" orientation="landscape" r:id="rId1"/>
   <rowBreaks count="1" manualBreakCount="1">
-    <brk id="27" max="16383" man="1"/>
+    <brk id="28" max="16383" man="1"/>
   </rowBreaks>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C2EC4BDB8795B64384668F447B3B8AC2" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="174724077d8640c2d7da640991664513">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="382902788bdcfee865055680d99b50db">
     <xsd:element name="properties">
@@ -1607,6 +1638,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -1617,21 +1654,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2073C62B-EE47-471C-AC82-37C409492412}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B4D7B7E3-993D-44C3-A68C-A03D50A3FA10}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1647,6 +1669,21 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2073C62B-EE47-471C-AC82-37C409492412}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F9A739D-B4C8-4DCE-A178-A71B36AE5162}">
   <ds:schemaRefs>

</xml_diff>